<commit_message>
Update the Test Pool Excel and pool.py files
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Week 3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Week 4" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Week 5" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Template Copy" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1506,8 +1505,8 @@
     <col width="13" customWidth="1" style="39" min="18" max="18"/>
     <col width="5.21875" customWidth="1" style="39" min="19" max="19"/>
     <col width="5" customWidth="1" style="39" min="20" max="20"/>
-    <col width="8.77734375" customWidth="1" style="39" min="21" max="22"/>
-    <col width="8.77734375" customWidth="1" style="39" min="23" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="21" max="25"/>
+    <col width="8.77734375" customWidth="1" style="39" min="26" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
@@ -2633,8 +2632,8 @@
     <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
     <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
     <col width="14.33203125" customWidth="1" style="39" min="18" max="19"/>
-    <col width="8.77734375" customWidth="1" style="39" min="20" max="21"/>
-    <col width="8.77734375" customWidth="1" style="39" min="22" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="20" max="24"/>
+    <col width="8.77734375" customWidth="1" style="39" min="25" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
@@ -3781,8 +3780,8 @@
     <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
     <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
     <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
-    <col width="8.77734375" customWidth="1" style="39" min="18" max="19"/>
-    <col width="8.77734375" customWidth="1" style="39" min="20" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="18" max="22"/>
+    <col width="8.77734375" customWidth="1" style="39" min="23" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
@@ -4893,8 +4892,8 @@
     <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
     <col width="14.33203125" customWidth="1" style="43" min="17" max="17"/>
     <col width="12.5546875" customWidth="1" style="39" min="18" max="18"/>
-    <col width="8.77734375" customWidth="1" style="39" min="19" max="20"/>
-    <col width="8.77734375" customWidth="1" style="39" min="21" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="19" max="23"/>
+    <col width="8.77734375" customWidth="1" style="39" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
@@ -5946,24 +5945,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Update Test Excel and pool.py file. Add fill color for player result cells for SNF and MNF.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4770" yWindow="2685" windowWidth="28800" windowHeight="11370" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -62,7 +62,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -117,6 +117,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000B0F0"/>
+        <bgColor rgb="0000B0F0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -467,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -669,6 +675,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,20 +1064,23 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="2"/>
-    <col width="17.44140625" customWidth="1" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" min="4" max="4"/>
-    <col width="17.44140625" customWidth="1" min="5" max="5"/>
+    <col width="17.453125" customWidth="1" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" min="4" max="4"/>
+    <col width="17.453125" customWidth="1" min="5" max="5"/>
     <col width="4" customWidth="1" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="1.90625" customWidth="1" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="5" customWidth="1" min="10" max="10"/>
+    <col width="5.453125" customWidth="1" min="11" max="11"/>
     <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" min="14" max="15"/>
+    <col width="1.90625" customWidth="1" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" min="14" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customHeight="1" thickBot="1">
+    <row r="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1487,31 +1502,31 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="14.44140625" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.109375" customWidth="1" style="39" min="5" max="5"/>
+    <col width="14.453125" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.08984375" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
-    <col width="14.5546875" customWidth="1" style="43" min="17" max="17"/>
+    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.81640625" customWidth="1" style="43" min="16" max="16"/>
+    <col width="14.54296875" customWidth="1" style="43" min="17" max="17"/>
     <col width="13" customWidth="1" style="39" min="18" max="18"/>
-    <col width="5.21875" customWidth="1" style="39" min="19" max="19"/>
+    <col width="5.1796875" customWidth="1" style="39" min="19" max="19"/>
     <col width="5" customWidth="1" style="39" min="20" max="20"/>
-    <col width="8.77734375" customWidth="1" style="39" min="21" max="30"/>
-    <col width="8.77734375" customWidth="1" style="39" min="31" max="16384"/>
+    <col width="8.81640625" customWidth="1" style="39" min="21" max="40"/>
+    <col width="8.81640625" customWidth="1" style="39" min="41" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -2493,7 +2508,7 @@
       <c r="P18" s="58" t="n"/>
       <c r="Q18" s="58" t="n"/>
     </row>
-    <row r="19" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="19" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -2559,7 +2574,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="21" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A21" s="34" t="inlineStr">
         <is>
           <t>playing against the</t>
@@ -2617,28 +2632,28 @@
       <selection activeCell="L19" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="13.44140625" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.21875" customWidth="1" style="39" min="5" max="5"/>
+    <col width="13.453125" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.1796875" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
-    <col width="14.33203125" customWidth="1" style="39" min="18" max="19"/>
-    <col width="8.77734375" customWidth="1" style="39" min="20" max="29"/>
-    <col width="8.77734375" customWidth="1" style="39" min="30" max="16384"/>
+    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.81640625" customWidth="1" style="43" min="16" max="17"/>
+    <col width="14.36328125" customWidth="1" style="39" min="18" max="19"/>
+    <col width="8.81640625" customWidth="1" style="39" min="20" max="39"/>
+    <col width="8.81640625" customWidth="1" style="39" min="40" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -3766,27 +3781,27 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="14.21875" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
-    <col width="13.88671875" customWidth="1" style="39" min="5" max="5"/>
+    <col width="14.1796875" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
+    <col width="13.90625" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
-    <col width="8.77734375" customWidth="1" style="39" min="18" max="27"/>
-    <col width="8.77734375" customWidth="1" style="39" min="28" max="16384"/>
+    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.81640625" customWidth="1" style="43" min="16" max="17"/>
+    <col width="8.81640625" customWidth="1" style="39" min="18" max="37"/>
+    <col width="8.81640625" customWidth="1" style="39" min="38" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -4873,32 +4888,32 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="13.44140625" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.21875" customWidth="1" style="39" min="5" max="5"/>
+    <col width="13.453125" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.1796875" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
-    <col width="14.33203125" customWidth="1" style="43" min="17" max="17"/>
-    <col width="12.5546875" customWidth="1" style="39" min="18" max="18"/>
-    <col width="8.77734375" customWidth="1" style="39" min="19" max="28"/>
-    <col width="8.77734375" customWidth="1" style="39" min="29" max="16384"/>
+    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.81640625" customWidth="1" style="43" min="16" max="16"/>
+    <col width="14.36328125" customWidth="1" style="43" min="17" max="17"/>
+    <col width="12.54296875" customWidth="1" style="39" min="18" max="18"/>
+    <col width="8.81640625" customWidth="1" style="39" min="19" max="38"/>
+    <col width="8.81640625" customWidth="1" style="39" min="39" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -5959,20 +5974,23 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="2"/>
-    <col width="17.44140625" customWidth="1" min="3" max="3"/>
-    <col width="6.44140625" customWidth="1" min="4" max="4"/>
-    <col width="17.44140625" customWidth="1" min="5" max="5"/>
+    <col width="17.453125" customWidth="1" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" min="4" max="4"/>
+    <col width="17.453125" customWidth="1" min="5" max="5"/>
     <col width="4" customWidth="1" min="6" max="7"/>
-    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="1.90625" customWidth="1" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="5" customWidth="1" min="10" max="10"/>
+    <col width="5.453125" customWidth="1" min="11" max="11"/>
     <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="1.88671875" customWidth="1" min="13" max="13"/>
-    <col width="7.109375" customWidth="1" min="14" max="15"/>
+    <col width="1.90625" customWidth="1" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" min="14" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customHeight="1" thickBot="1">
+    <row r="1" ht="16.2" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6473,8 +6491,8 @@
       </c>
       <c r="L14" s="17" t="n"/>
       <c r="M14" s="18" t="n"/>
-      <c r="N14" s="24" t="n"/>
-      <c r="O14" s="24" t="n"/>
+      <c r="N14" s="87" t="n"/>
+      <c r="O14" s="87" t="n"/>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="15" t="n"/>
@@ -6508,8 +6526,8 @@
       </c>
       <c r="L15" s="17" t="n"/>
       <c r="M15" s="18" t="n"/>
-      <c r="N15" s="61" t="n"/>
-      <c r="O15" s="19" t="n"/>
+      <c r="N15" s="88" t="n"/>
+      <c r="O15" s="87" t="n"/>
     </row>
     <row r="16" ht="15.6" customHeight="1">
       <c r="A16" s="15" t="n"/>

</xml_diff>

<commit_message>
Updates to get apply home team color fill in cell.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Week 3" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Week 4" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Week 5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Week 6" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -6650,4 +6651,676 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="2"/>
+    <col width="17.453125" customWidth="1" min="3" max="3"/>
+    <col width="6.453125" customWidth="1" min="4" max="4"/>
+    <col width="17.453125" customWidth="1" min="5" max="5"/>
+    <col width="4" customWidth="1" min="6" max="7"/>
+    <col width="1.90625" customWidth="1" min="8" max="8"/>
+    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="5" customWidth="1" min="10" max="10"/>
+    <col width="5.453125" customWidth="1" min="11" max="11"/>
+    <col width="5" customWidth="1" min="12" max="12"/>
+    <col width="1.90625" customWidth="1" min="13" max="13"/>
+    <col width="7.08984375" customWidth="1" min="14" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.2" customHeight="1" thickBot="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="C1" s="73" t="inlineStr">
+        <is>
+          <t>AMERICA'S LINE</t>
+        </is>
+      </c>
+      <c r="D1" s="74" t="n"/>
+      <c r="E1" s="75" t="n"/>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="n"/>
+      <c r="I1" s="76" t="inlineStr">
+        <is>
+          <t>ACTUAL SCORES</t>
+        </is>
+      </c>
+      <c r="J1" s="74" t="n"/>
+      <c r="K1" s="74" t="n"/>
+      <c r="L1" s="75" t="n"/>
+      <c r="M1" s="11" t="n"/>
+      <c r="N1" s="12" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="O1" s="13" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.6" customHeight="1">
+      <c r="A2" s="15" t="n"/>
+      <c r="B2" s="15" t="n"/>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>PANTHERS</t>
+        </is>
+      </c>
+      <c r="D2" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>BEARS</t>
+        </is>
+      </c>
+      <c r="F2" s="55" t="n"/>
+      <c r="G2" s="55" t="n"/>
+      <c r="H2" s="16" t="n"/>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>CAR</t>
+        </is>
+      </c>
+      <c r="J2" s="17" t="n"/>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="L2" s="17" t="n"/>
+      <c r="M2" s="18" t="n"/>
+      <c r="N2" s="61" t="n"/>
+      <c r="O2" s="70" t="n"/>
+    </row>
+    <row r="3" ht="15.6" customHeight="1">
+      <c r="A3" s="15" t="n"/>
+      <c r="B3" s="15" t="n"/>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>LIONS</t>
+        </is>
+      </c>
+      <c r="D3" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>JAGUARS</t>
+        </is>
+      </c>
+      <c r="F3" s="21" t="n"/>
+      <c r="G3" s="15" t="n"/>
+      <c r="H3" s="16" t="n"/>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="J3" s="17" t="n"/>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>JAX</t>
+        </is>
+      </c>
+      <c r="L3" s="17" t="n"/>
+      <c r="M3" s="18" t="n"/>
+      <c r="N3" s="61" t="n"/>
+      <c r="O3" s="19" t="n"/>
+    </row>
+    <row r="4" ht="15.6" customHeight="1">
+      <c r="A4" s="15" t="n"/>
+      <c r="B4" s="15" t="n"/>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>VIKINGS</t>
+        </is>
+      </c>
+      <c r="D4" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>FALCONS</t>
+        </is>
+      </c>
+      <c r="F4" s="21" t="n"/>
+      <c r="G4" s="15" t="n"/>
+      <c r="H4" s="16" t="n"/>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="J4" s="17" t="n"/>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="L4" s="17" t="n"/>
+      <c r="M4" s="18" t="n"/>
+      <c r="N4" s="61" t="n"/>
+      <c r="O4" s="19" t="n"/>
+    </row>
+    <row r="5" ht="15.6" customHeight="1">
+      <c r="A5" s="15" t="n"/>
+      <c r="B5" s="15" t="n"/>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>TEXANS</t>
+        </is>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>TITANS</t>
+        </is>
+      </c>
+      <c r="F5" s="21" t="n"/>
+      <c r="G5" s="15" t="n"/>
+      <c r="H5" s="16" t="n"/>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="J5" s="17" t="n"/>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>TEN</t>
+        </is>
+      </c>
+      <c r="L5" s="17" t="n"/>
+      <c r="M5" s="18" t="n"/>
+      <c r="N5" s="61" t="n"/>
+      <c r="O5" s="19" t="n"/>
+    </row>
+    <row r="6" ht="15.6" customHeight="1">
+      <c r="A6" s="15" t="n"/>
+      <c r="B6" s="15" t="n"/>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>GIANTS</t>
+        </is>
+      </c>
+      <c r="D6" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>FOOTBALL TEAM</t>
+        </is>
+      </c>
+      <c r="F6" s="21" t="n"/>
+      <c r="G6" s="15" t="n"/>
+      <c r="H6" s="16" t="n"/>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>NYG</t>
+        </is>
+      </c>
+      <c r="J6" s="17" t="n"/>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="L6" s="17" t="n"/>
+      <c r="M6" s="18" t="n"/>
+      <c r="N6" s="61" t="n"/>
+      <c r="O6" s="19" t="n"/>
+    </row>
+    <row r="7" ht="15.6" customHeight="1">
+      <c r="A7" s="15" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>STEELERS</t>
+        </is>
+      </c>
+      <c r="D7" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>BROWNS</t>
+        </is>
+      </c>
+      <c r="F7" s="21" t="n"/>
+      <c r="G7" s="15" t="n"/>
+      <c r="H7" s="16" t="n"/>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="J7" s="17" t="n"/>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="L7" s="17" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="61" t="n"/>
+      <c r="O7" s="61" t="n"/>
+    </row>
+    <row r="8" ht="15.6" customHeight="1">
+      <c r="A8" s="15" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>RAVENS</t>
+        </is>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>EAGLES</t>
+        </is>
+      </c>
+      <c r="F8" s="57" t="n"/>
+      <c r="G8" s="15" t="n"/>
+      <c r="H8" s="16" t="n"/>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>BAL</t>
+        </is>
+      </c>
+      <c r="J8" s="17" t="n"/>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="L8" s="17" t="n"/>
+      <c r="M8" s="18" t="n"/>
+      <c r="N8" s="61" t="n"/>
+      <c r="O8" s="19" t="n"/>
+    </row>
+    <row r="9" ht="15.6" customHeight="1">
+      <c r="A9" s="15" t="n"/>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>COLTS</t>
+        </is>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>BENGALS</t>
+        </is>
+      </c>
+      <c r="F9" s="21" t="n"/>
+      <c r="G9" s="15" t="n"/>
+      <c r="H9" s="16" t="n"/>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="J9" s="17" t="n"/>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="L9" s="17" t="n"/>
+      <c r="M9" s="18" t="n"/>
+      <c r="N9" s="61" t="n"/>
+      <c r="O9" s="19" t="n"/>
+    </row>
+    <row r="10" ht="15.6" customHeight="1">
+      <c r="A10" s="15" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>BRONCOS</t>
+        </is>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>PATRIOTS</t>
+        </is>
+      </c>
+      <c r="F10" s="21" t="n"/>
+      <c r="G10" s="15" t="n"/>
+      <c r="H10" s="16" t="n"/>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="J10" s="17" t="n"/>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="L10" s="17" t="n"/>
+      <c r="M10" s="18" t="n"/>
+      <c r="N10" s="61" t="n"/>
+      <c r="O10" s="19" t="n"/>
+    </row>
+    <row r="11" ht="15.6" customHeight="1">
+      <c r="A11" s="15" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>DOLPHINS</t>
+        </is>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>JETS</t>
+        </is>
+      </c>
+      <c r="F11" s="57" t="n"/>
+      <c r="G11" s="15" t="n"/>
+      <c r="H11" s="16" t="n"/>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="J11" s="17" t="n"/>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>NYJ</t>
+        </is>
+      </c>
+      <c r="L11" s="17" t="n"/>
+      <c r="M11" s="18" t="n"/>
+      <c r="N11" s="61" t="n"/>
+      <c r="O11" s="19" t="n"/>
+    </row>
+    <row r="12" ht="15.6" customHeight="1">
+      <c r="A12" s="15" t="n"/>
+      <c r="B12" s="15" t="n"/>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>PACKERS</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>BUCCANEERS</t>
+        </is>
+      </c>
+      <c r="F12" s="21" t="n"/>
+      <c r="G12" s="15" t="n"/>
+      <c r="H12" s="16" t="n"/>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="J12" s="17" t="n"/>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="L12" s="17" t="n"/>
+      <c r="M12" s="18" t="n"/>
+      <c r="N12" s="61" t="n"/>
+      <c r="O12" s="19" t="n"/>
+    </row>
+    <row r="13" ht="15.6" customHeight="1">
+      <c r="A13" s="15" t="n"/>
+      <c r="B13" s="15" t="n"/>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>RAMS</t>
+        </is>
+      </c>
+      <c r="D13" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>49ERS</t>
+        </is>
+      </c>
+      <c r="F13" s="21" t="n"/>
+      <c r="G13" s="15" t="n"/>
+      <c r="H13" s="16" t="n"/>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>LAR</t>
+        </is>
+      </c>
+      <c r="J13" s="17" t="n"/>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="L13" s="17" t="n"/>
+      <c r="M13" s="18" t="n"/>
+      <c r="N13" s="88" t="n"/>
+      <c r="O13" s="87" t="n"/>
+    </row>
+    <row r="14" ht="15.6" customHeight="1">
+      <c r="A14" s="15" t="n"/>
+      <c r="B14" s="15" t="n"/>
+      <c r="C14" s="4" t="inlineStr">
+        <is>
+          <t>CHIEFS</t>
+        </is>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="inlineStr">
+        <is>
+          <t>BILLS</t>
+        </is>
+      </c>
+      <c r="F14" s="21" t="n"/>
+      <c r="G14" s="15" t="n"/>
+      <c r="H14" s="16" t="n"/>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>KC</t>
+        </is>
+      </c>
+      <c r="J14" s="17" t="n"/>
+      <c r="K14" s="5" t="inlineStr">
+        <is>
+          <t>BUF</t>
+        </is>
+      </c>
+      <c r="L14" s="17" t="n"/>
+      <c r="M14" s="18" t="n"/>
+      <c r="N14" s="87" t="n"/>
+      <c r="O14" s="87" t="n"/>
+    </row>
+    <row r="15" ht="15.6" customHeight="1">
+      <c r="A15" s="15" t="n"/>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="4" t="n"/>
+      <c r="D15" s="15" t="n"/>
+      <c r="E15" s="4" t="n"/>
+      <c r="F15" s="21" t="n"/>
+      <c r="G15" s="15" t="n"/>
+      <c r="H15" s="16" t="n"/>
+      <c r="I15" s="2" t="n"/>
+      <c r="J15" s="17" t="n"/>
+      <c r="K15" s="2" t="n"/>
+      <c r="L15" s="17" t="n"/>
+      <c r="M15" s="18" t="n"/>
+      <c r="N15" s="61" t="n"/>
+      <c r="O15" s="19" t="n"/>
+    </row>
+    <row r="16" ht="15.6" customHeight="1">
+      <c r="A16" s="15" t="n"/>
+      <c r="B16" s="15" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="15" t="n"/>
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="21" t="n"/>
+      <c r="G16" s="15" t="n"/>
+      <c r="H16" s="16" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="17" t="n"/>
+      <c r="M16" s="18" t="n"/>
+      <c r="N16" s="24" t="n"/>
+      <c r="O16" s="24" t="n"/>
+    </row>
+    <row r="17" ht="15.6" customHeight="1">
+      <c r="A17" s="15" t="n"/>
+      <c r="B17" s="15" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="21" t="n"/>
+      <c r="G17" s="15" t="n"/>
+      <c r="H17" s="16" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="17" t="n"/>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="17" t="n"/>
+      <c r="M17" s="18" t="n"/>
+      <c r="N17" s="61" t="n"/>
+      <c r="O17" s="19" t="n"/>
+    </row>
+    <row r="18" ht="15.6" customHeight="1">
+      <c r="A18" s="26" t="n"/>
+      <c r="B18" s="26" t="n"/>
+      <c r="C18" s="67" t="n"/>
+      <c r="D18" s="56" t="n"/>
+      <c r="E18" s="68" t="n"/>
+      <c r="F18" s="28" t="n"/>
+      <c r="G18" s="26" t="n"/>
+      <c r="H18" s="29" t="n"/>
+      <c r="I18" s="5" t="n"/>
+      <c r="J18" s="17" t="n"/>
+      <c r="K18" s="5" t="n"/>
+      <c r="L18" s="17" t="inlineStr">
+        <is>
+          <t>SUB</t>
+        </is>
+      </c>
+      <c r="M18" s="16" t="n"/>
+      <c r="N18" s="19" t="n"/>
+      <c r="O18" s="19" t="n"/>
+    </row>
+    <row r="19" ht="15.6" customHeight="1">
+      <c r="A19" s="26" t="n"/>
+      <c r="B19" s="26" t="n"/>
+      <c r="C19" s="67" t="n"/>
+      <c r="D19" s="56" t="n"/>
+      <c r="E19" s="68" t="n"/>
+      <c r="F19" s="28" t="n"/>
+      <c r="G19" s="26" t="n"/>
+      <c r="H19" s="29" t="n"/>
+      <c r="I19" s="5" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="5" t="n"/>
+      <c r="L19" s="17" t="inlineStr">
+        <is>
+          <t>WK</t>
+        </is>
+      </c>
+      <c r="M19" s="16" t="n"/>
+      <c r="N19" s="19" t="n"/>
+      <c r="O19" s="19" t="n"/>
+    </row>
+    <row r="20" ht="15.6" customHeight="1">
+      <c r="A20" s="26" t="n"/>
+      <c r="B20" s="26" t="n"/>
+      <c r="C20" s="67" t="n"/>
+      <c r="D20" s="56" t="n"/>
+      <c r="E20" s="68" t="n"/>
+      <c r="F20" s="28" t="n"/>
+      <c r="G20" s="26" t="n"/>
+      <c r="H20" s="29" t="n"/>
+      <c r="I20" s="5" t="n"/>
+      <c r="J20" s="17" t="n"/>
+      <c r="K20" s="5" t="n"/>
+      <c r="L20" s="31" t="inlineStr">
+        <is>
+          <t>YTD</t>
+        </is>
+      </c>
+      <c r="M20" s="16" t="n"/>
+      <c r="N20" s="19" t="n"/>
+      <c r="O20" s="19" t="n"/>
+    </row>
+    <row r="21" ht="15.6" customHeight="1">
+      <c r="A21" s="61" t="n"/>
+      <c r="B21" s="61" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="69" t="n"/>
+      <c r="G21" s="61" t="n"/>
+      <c r="H21" s="16" t="n"/>
+      <c r="I21" s="5" t="n"/>
+      <c r="J21" s="17" t="n"/>
+      <c r="K21" s="5" t="n"/>
+      <c r="L21" s="17" t="n"/>
+      <c r="M21" s="16" t="n"/>
+      <c r="N21" s="19" t="n"/>
+      <c r="O21" s="19" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Test Excel and pool.py files. Fill home team's cell with color.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -63,7 +63,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -116,6 +116,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4B084"/>
+        <bgColor rgb="00F4B084"/>
       </patternFill>
     </fill>
     <fill>
@@ -474,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -649,6 +661,12 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -676,10 +694,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1065,23 +1093,23 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="2"/>
-    <col width="17.453125" customWidth="1" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" min="4" max="4"/>
-    <col width="17.453125" customWidth="1" min="5" max="5"/>
+    <col width="17.44140625" customWidth="1" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" min="4" max="4"/>
+    <col width="17.44140625" customWidth="1" min="5" max="5"/>
     <col width="4" customWidth="1" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" min="11" max="11"/>
     <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" min="14" max="15"/>
+    <col width="1.88671875" customWidth="1" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" min="14" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customHeight="1" thickBot="1">
+    <row r="1" ht="16.15" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1092,13 +1120,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="73" t="inlineStr">
+      <c r="C1" s="75" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="74" t="n"/>
-      <c r="E1" s="75" t="n"/>
+      <c r="D1" s="76" t="n"/>
+      <c r="E1" s="77" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1110,14 +1138,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="76" t="inlineStr">
+      <c r="I1" s="78" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="74" t="n"/>
-      <c r="K1" s="74" t="n"/>
-      <c r="L1" s="75" t="n"/>
+      <c r="J1" s="76" t="n"/>
+      <c r="K1" s="76" t="n"/>
+      <c r="L1" s="77" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -1503,31 +1531,31 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="14.453125" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.08984375" customWidth="1" style="39" min="5" max="5"/>
+    <col width="14.44140625" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.109375" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.81640625" customWidth="1" style="43" min="16" max="16"/>
-    <col width="14.54296875" customWidth="1" style="43" min="17" max="17"/>
+    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
+    <col width="14.5546875" customWidth="1" style="43" min="17" max="17"/>
     <col width="13" customWidth="1" style="39" min="18" max="18"/>
-    <col width="5.1796875" customWidth="1" style="39" min="19" max="19"/>
+    <col width="5.21875" customWidth="1" style="39" min="19" max="19"/>
     <col width="5" customWidth="1" style="39" min="20" max="20"/>
-    <col width="8.81640625" customWidth="1" style="39" min="21" max="40"/>
-    <col width="8.81640625" customWidth="1" style="39" min="41" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="21" max="46"/>
+    <col width="8.77734375" customWidth="1" style="39" min="47" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1538,13 +1566,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="77" t="inlineStr">
+      <c r="C1" s="79" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="78" t="n"/>
-      <c r="E1" s="79" t="n"/>
+      <c r="D1" s="80" t="n"/>
+      <c r="E1" s="81" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1556,14 +1584,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="80" t="inlineStr">
+      <c r="I1" s="82" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="78" t="n"/>
-      <c r="K1" s="78" t="n"/>
-      <c r="L1" s="81" t="n"/>
+      <c r="J1" s="80" t="n"/>
+      <c r="K1" s="80" t="n"/>
+      <c r="L1" s="83" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -1578,7 +1606,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A2" s="15" t="n"/>
       <c r="B2" s="15" t="n"/>
       <c r="C2" s="22" t="inlineStr">
@@ -1634,7 +1662,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1690,7 +1718,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1746,7 +1774,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1802,7 +1830,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -1858,7 +1886,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A7" s="15" t="n"/>
       <c r="B7" s="15" t="n"/>
       <c r="C7" s="23" t="inlineStr">
@@ -1912,13 +1940,13 @@
           <t>W</t>
         </is>
       </c>
-      <c r="P7" s="85" t="inlineStr">
+      <c r="P7" s="87" t="inlineStr">
         <is>
           <t>De predicts 49ers 27-20</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1974,7 +2002,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2030,7 +2058,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2086,7 +2114,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A11" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2142,7 +2170,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2198,7 +2226,7 @@
       </c>
       <c r="P12" s="58" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A13" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2254,7 +2282,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2310,7 +2338,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2366,7 +2394,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A16" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2422,7 +2450,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A17" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2478,7 +2506,7 @@
       </c>
       <c r="P17" s="58" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -2509,7 +2537,7 @@
       <c r="P18" s="58" t="n"/>
       <c r="Q18" s="58" t="n"/>
     </row>
-    <row r="19" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="19" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -2540,20 +2568,20 @@
       <c r="P19" s="58" t="n"/>
       <c r="Q19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="86">
-      <c r="A20" s="82" t="inlineStr">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
+      <c r="A20" s="84" t="inlineStr">
         <is>
           <t>DeM says the Super Bowl will be won by the Falcons</t>
         </is>
       </c>
-      <c r="B20" s="83" t="n"/>
-      <c r="C20" s="83" t="n"/>
-      <c r="D20" s="83" t="n"/>
-      <c r="E20" s="83" t="n"/>
-      <c r="F20" s="83" t="n"/>
-      <c r="G20" s="83" t="n"/>
-      <c r="H20" s="83" t="n"/>
-      <c r="I20" s="84" t="n"/>
+      <c r="B20" s="85" t="n"/>
+      <c r="C20" s="85" t="n"/>
+      <c r="D20" s="85" t="n"/>
+      <c r="E20" s="85" t="n"/>
+      <c r="F20" s="85" t="n"/>
+      <c r="G20" s="85" t="n"/>
+      <c r="H20" s="85" t="n"/>
+      <c r="I20" s="86" t="n"/>
       <c r="J20" s="31" t="n"/>
       <c r="K20" s="27" t="n"/>
       <c r="L20" s="31" t="inlineStr">
@@ -2575,7 +2603,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="21" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A21" s="34" t="inlineStr">
         <is>
           <t>playing against the</t>
@@ -2633,28 +2661,28 @@
       <selection activeCell="L19" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="13.453125" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.1796875" customWidth="1" style="39" min="5" max="5"/>
+    <col width="13.44140625" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.21875" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.81640625" customWidth="1" style="43" min="16" max="17"/>
-    <col width="14.36328125" customWidth="1" style="39" min="18" max="19"/>
-    <col width="8.81640625" customWidth="1" style="39" min="20" max="39"/>
-    <col width="8.81640625" customWidth="1" style="39" min="40" max="16384"/>
+    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
+    <col width="14.33203125" customWidth="1" style="39" min="18" max="19"/>
+    <col width="8.77734375" customWidth="1" style="39" min="20" max="45"/>
+    <col width="8.77734375" customWidth="1" style="39" min="46" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -2665,13 +2693,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="77" t="inlineStr">
+      <c r="C1" s="79" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="78" t="n"/>
-      <c r="E1" s="79" t="n"/>
+      <c r="D1" s="80" t="n"/>
+      <c r="E1" s="81" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -2683,14 +2711,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="80" t="inlineStr">
+      <c r="I1" s="82" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="78" t="n"/>
-      <c r="K1" s="78" t="n"/>
-      <c r="L1" s="81" t="n"/>
+      <c r="J1" s="80" t="n"/>
+      <c r="K1" s="80" t="n"/>
+      <c r="L1" s="83" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -2705,7 +2733,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A2" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2761,7 +2789,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2817,7 +2845,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A4" s="15" t="n"/>
       <c r="B4" s="15" t="inlineStr">
         <is>
@@ -2873,7 +2901,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2929,7 +2957,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -2985,7 +3013,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3041,7 +3069,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3097,7 +3125,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3153,7 +3181,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3209,7 +3237,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
       <c r="C11" s="20" t="inlineStr">
@@ -3276,7 +3304,7 @@
       <c r="V11" s="58" t="n"/>
       <c r="W11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3343,7 +3371,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A13" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3410,7 +3438,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3466,7 +3494,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3522,7 +3550,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A16" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3578,7 +3606,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A17" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3634,7 +3662,7 @@
       </c>
       <c r="P17" s="58" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -3665,7 +3693,7 @@
       <c r="P18" s="58" t="n"/>
       <c r="Q18" s="45" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -3699,7 +3727,7 @@
       <c r="S19" s="46" t="n"/>
       <c r="T19" s="46" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -3730,7 +3758,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="C21" s="27" t="n"/>
@@ -3782,27 +3810,27 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="14.1796875" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
-    <col width="13.90625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="14.21875" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
+    <col width="13.88671875" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.81640625" customWidth="1" style="43" min="16" max="17"/>
-    <col width="8.81640625" customWidth="1" style="39" min="18" max="37"/>
-    <col width="8.81640625" customWidth="1" style="39" min="38" max="16384"/>
+    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
+    <col width="8.77734375" customWidth="1" style="39" min="18" max="43"/>
+    <col width="8.77734375" customWidth="1" style="39" min="44" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -3813,13 +3841,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="77" t="inlineStr">
+      <c r="C1" s="79" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="78" t="n"/>
-      <c r="E1" s="79" t="n"/>
+      <c r="D1" s="80" t="n"/>
+      <c r="E1" s="81" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -3831,14 +3859,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="80" t="inlineStr">
+      <c r="I1" s="82" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="78" t="n"/>
-      <c r="K1" s="78" t="n"/>
-      <c r="L1" s="81" t="n"/>
+      <c r="J1" s="80" t="n"/>
+      <c r="K1" s="80" t="n"/>
+      <c r="L1" s="83" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -3853,7 +3881,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A2" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -3909,7 +3937,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A3" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -3965,7 +3993,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A4" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4021,7 +4049,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A5" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4077,7 +4105,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A6" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4133,7 +4161,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A7" s="61" t="n"/>
       <c r="B7" s="61" t="inlineStr">
         <is>
@@ -4189,7 +4217,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A8" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4245,7 +4273,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A9" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4301,7 +4329,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A10" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4357,7 +4385,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A11" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4413,7 +4441,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A12" s="61" t="n"/>
       <c r="B12" s="61" t="inlineStr">
         <is>
@@ -4469,7 +4497,7 @@
       </c>
       <c r="P12" s="58" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A13" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4525,7 +4553,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A14" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4581,7 +4609,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A15" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4637,7 +4665,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A16" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4693,7 +4721,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A17" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4751,7 +4779,7 @@
       <c r="Q17" s="66" t="n"/>
       <c r="R17" s="66" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -4781,7 +4809,7 @@
       </c>
       <c r="P18" s="58" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -4812,7 +4840,7 @@
       <c r="P19" s="58" t="n"/>
       <c r="Q19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -4843,7 +4871,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="D21" s="26" t="n"/>
@@ -4888,33 +4916,33 @@
   </sheetPr>
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.81640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" style="39" min="1" max="2"/>
-    <col width="13.453125" customWidth="1" style="39" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" style="40" min="4" max="4"/>
-    <col width="14.1796875" customWidth="1" style="39" min="5" max="5"/>
+    <col width="13.44140625" customWidth="1" style="39" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" style="40" min="4" max="4"/>
+    <col width="14.21875" customWidth="1" style="39" min="5" max="5"/>
     <col width="4" customWidth="1" style="39" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" style="39" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" style="39" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" style="39" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" style="39" min="9" max="9"/>
     <col width="5" customWidth="1" style="39" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" style="39" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" style="39" min="11" max="11"/>
     <col width="5" customWidth="1" style="39" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" style="39" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" style="41" min="14" max="14"/>
-    <col width="7.08984375" customWidth="1" style="42" min="15" max="15"/>
-    <col width="8.81640625" customWidth="1" style="43" min="16" max="16"/>
-    <col width="14.36328125" customWidth="1" style="43" min="17" max="17"/>
-    <col width="12.54296875" customWidth="1" style="39" min="18" max="18"/>
-    <col width="8.81640625" customWidth="1" style="39" min="19" max="38"/>
-    <col width="8.81640625" customWidth="1" style="39" min="39" max="16384"/>
+    <col width="1.88671875" customWidth="1" style="39" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
+    <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
+    <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
+    <col width="14.33203125" customWidth="1" style="43" min="17" max="17"/>
+    <col width="12.5546875" customWidth="1" style="39" min="18" max="18"/>
+    <col width="8.77734375" customWidth="1" style="39" min="19" max="44"/>
+    <col width="8.77734375" customWidth="1" style="39" min="45" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customFormat="1" customHeight="1" s="86" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -4925,13 +4953,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="77" t="inlineStr">
+      <c r="C1" s="79" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="78" t="n"/>
-      <c r="E1" s="79" t="n"/>
+      <c r="D1" s="80" t="n"/>
+      <c r="E1" s="81" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -4943,14 +4971,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="80" t="inlineStr">
+      <c r="I1" s="82" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="78" t="n"/>
-      <c r="K1" s="78" t="n"/>
-      <c r="L1" s="81" t="n"/>
+      <c r="J1" s="80" t="n"/>
+      <c r="K1" s="80" t="n"/>
+      <c r="L1" s="83" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -4965,7 +4993,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A2" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5021,7 +5049,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5077,7 +5105,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A4" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5133,7 +5161,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A5" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5189,7 +5217,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A6" s="61" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -5245,7 +5273,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A7" s="61" t="n"/>
       <c r="B7" s="15" t="inlineStr">
         <is>
@@ -5301,7 +5329,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5357,7 +5385,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A9" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5413,7 +5441,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A10" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5469,7 +5497,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A11" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5525,7 +5553,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A12" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5582,7 +5610,7 @@
       <c r="P12" s="58" t="n"/>
       <c r="T12" s="46" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A13" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5638,7 +5666,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5694,7 +5722,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5750,7 +5778,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A16" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5806,7 +5834,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A17" s="15" t="n"/>
       <c r="B17" s="15" t="n"/>
       <c r="C17" s="1" t="n"/>
@@ -5827,7 +5855,7 @@
       <c r="R17" s="66" t="n"/>
       <c r="T17" s="46" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -5857,7 +5885,7 @@
       </c>
       <c r="P18" s="58" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -5887,7 +5915,7 @@
       </c>
       <c r="P19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -5917,7 +5945,7 @@
       </c>
       <c r="P20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="86">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="C21" s="27" t="n"/>
@@ -5971,27 +5999,27 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="2"/>
-    <col width="17.453125" customWidth="1" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" min="4" max="4"/>
-    <col width="17.453125" customWidth="1" min="5" max="5"/>
+    <col width="17.44140625" customWidth="1" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" min="4" max="4"/>
+    <col width="17.44140625" customWidth="1" min="5" max="5"/>
     <col width="4" customWidth="1" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" min="11" max="11"/>
     <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" min="14" max="15"/>
+    <col width="1.88671875" customWidth="1" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" min="14" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customHeight="1" thickBot="1">
+    <row r="1" ht="16.15" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6002,13 +6030,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="73" t="inlineStr">
+      <c r="C1" s="75" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="74" t="n"/>
-      <c r="E1" s="75" t="n"/>
+      <c r="D1" s="76" t="n"/>
+      <c r="E1" s="77" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6020,14 +6048,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="76" t="inlineStr">
+      <c r="I1" s="78" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="74" t="n"/>
-      <c r="K1" s="74" t="n"/>
-      <c r="L1" s="75" t="n"/>
+      <c r="J1" s="76" t="n"/>
+      <c r="K1" s="76" t="n"/>
+      <c r="L1" s="77" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -6492,8 +6520,8 @@
       </c>
       <c r="L14" s="17" t="n"/>
       <c r="M14" s="18" t="n"/>
-      <c r="N14" s="87" t="n"/>
-      <c r="O14" s="87" t="n"/>
+      <c r="N14" s="72" t="n"/>
+      <c r="O14" s="72" t="n"/>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="15" t="n"/>
@@ -6527,8 +6555,8 @@
       </c>
       <c r="L15" s="17" t="n"/>
       <c r="M15" s="18" t="n"/>
-      <c r="N15" s="88" t="n"/>
-      <c r="O15" s="87" t="n"/>
+      <c r="N15" s="73" t="n"/>
+      <c r="O15" s="72" t="n"/>
     </row>
     <row r="16" ht="15.6" customHeight="1">
       <c r="A16" s="15" t="n"/>
@@ -6665,23 +6693,23 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="4" customWidth="1" min="1" max="2"/>
-    <col width="17.453125" customWidth="1" min="3" max="3"/>
-    <col width="6.453125" customWidth="1" min="4" max="4"/>
-    <col width="17.453125" customWidth="1" min="5" max="5"/>
+    <col width="17.44140625" customWidth="1" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" min="4" max="4"/>
+    <col width="17.44140625" customWidth="1" min="5" max="5"/>
     <col width="4" customWidth="1" min="6" max="7"/>
-    <col width="1.90625" customWidth="1" min="8" max="8"/>
-    <col width="5.453125" customWidth="1" min="9" max="9"/>
+    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
-    <col width="5.453125" customWidth="1" min="11" max="11"/>
+    <col width="5.44140625" customWidth="1" min="11" max="11"/>
     <col width="5" customWidth="1" min="12" max="12"/>
-    <col width="1.90625" customWidth="1" min="13" max="13"/>
-    <col width="7.08984375" customWidth="1" min="14" max="15"/>
+    <col width="1.88671875" customWidth="1" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" min="14" max="15"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.2" customHeight="1" thickBot="1">
+    <row r="1" ht="16.15" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6692,13 +6720,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="73" t="inlineStr">
+      <c r="C1" s="75" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="74" t="n"/>
-      <c r="E1" s="75" t="n"/>
+      <c r="D1" s="76" t="n"/>
+      <c r="E1" s="77" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6710,14 +6738,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="76" t="inlineStr">
+      <c r="I1" s="78" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="74" t="n"/>
-      <c r="K1" s="74" t="n"/>
-      <c r="L1" s="75" t="n"/>
+      <c r="J1" s="76" t="n"/>
+      <c r="K1" s="76" t="n"/>
+      <c r="L1" s="77" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -6733,7 +6761,7 @@
     <row r="2" ht="15.6" customHeight="1">
       <c r="A2" s="15" t="n"/>
       <c r="B2" s="15" t="n"/>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="89" t="inlineStr">
         <is>
           <t>PANTHERS</t>
         </is>
@@ -6776,7 +6804,7 @@
       <c r="D3" s="15" t="n">
         <v>3.5</v>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="89" t="inlineStr">
         <is>
           <t>JAGUARS</t>
         </is>
@@ -6803,7 +6831,7 @@
     <row r="4" ht="15.6" customHeight="1">
       <c r="A4" s="15" t="n"/>
       <c r="B4" s="15" t="n"/>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="90" t="inlineStr">
         <is>
           <t>VIKINGS</t>
         </is>
@@ -6838,17 +6866,17 @@
     <row r="5" ht="15.6" customHeight="1">
       <c r="A5" s="15" t="n"/>
       <c r="B5" s="15" t="n"/>
-      <c r="C5" s="1" t="inlineStr">
+      <c r="C5" s="91" t="inlineStr">
+        <is>
+          <t>TITANS</t>
+        </is>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>TEXANS</t>
-        </is>
-      </c>
-      <c r="D5" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>TITANS</t>
         </is>
       </c>
       <c r="F5" s="21" t="n"/>
@@ -6856,13 +6884,13 @@
       <c r="H5" s="16" t="n"/>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="J5" s="17" t="n"/>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="L5" s="17" t="n"/>
@@ -6873,7 +6901,7 @@
     <row r="6" ht="15.6" customHeight="1">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="n"/>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" s="92" t="inlineStr">
         <is>
           <t>GIANTS</t>
         </is>
@@ -6908,7 +6936,7 @@
     <row r="7" ht="15.6" customHeight="1">
       <c r="A7" s="15" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="C7" s="91" t="inlineStr">
         <is>
           <t>STEELERS</t>
         </is>
@@ -6951,7 +6979,7 @@
       <c r="D8" s="15" t="n">
         <v>7.5</v>
       </c>
-      <c r="E8" s="1" t="inlineStr">
+      <c r="E8" s="91" t="inlineStr">
         <is>
           <t>EAGLES</t>
         </is>
@@ -6978,7 +7006,7 @@
     <row r="9" ht="15.6" customHeight="1">
       <c r="A9" s="15" t="n"/>
       <c r="B9" s="15" t="n"/>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="92" t="inlineStr">
         <is>
           <t>COLTS</t>
         </is>
@@ -7013,17 +7041,17 @@
     <row r="10" ht="15.6" customHeight="1">
       <c r="A10" s="15" t="n"/>
       <c r="B10" s="15" t="n"/>
-      <c r="C10" s="1" t="inlineStr">
+      <c r="C10" s="91" t="inlineStr">
+        <is>
+          <t>PATRIOTS</t>
+        </is>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>BRONCOS</t>
-        </is>
-      </c>
-      <c r="D10" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
-        <is>
-          <t>PATRIOTS</t>
         </is>
       </c>
       <c r="F10" s="21" t="n"/>
@@ -7031,13 +7059,13 @@
       <c r="H10" s="16" t="n"/>
       <c r="I10" s="2" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="J10" s="17" t="n"/>
       <c r="K10" s="2" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="L10" s="17" t="n"/>
@@ -7048,13 +7076,13 @@
     <row r="11" ht="15.6" customHeight="1">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" s="92" t="inlineStr">
         <is>
           <t>DOLPHINS</t>
         </is>
       </c>
       <c r="D11" s="15" t="n">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="E11" s="4" t="inlineStr">
         <is>
@@ -7089,9 +7117,9 @@
         </is>
       </c>
       <c r="D12" s="15" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
+        <v>2</v>
+      </c>
+      <c r="E12" s="92" t="inlineStr">
         <is>
           <t>BUCCANEERS</t>
         </is>
@@ -7126,7 +7154,7 @@
       <c r="D13" s="15" t="n">
         <v>3.5</v>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="92" t="inlineStr">
         <is>
           <t>49ERS</t>
         </is>
@@ -7147,8 +7175,8 @@
       </c>
       <c r="L13" s="17" t="n"/>
       <c r="M13" s="18" t="n"/>
-      <c r="N13" s="88" t="n"/>
-      <c r="O13" s="87" t="n"/>
+      <c r="N13" s="93" t="n"/>
+      <c r="O13" s="94" t="n"/>
     </row>
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="15" t="n"/>
@@ -7159,9 +7187,9 @@
         </is>
       </c>
       <c r="D14" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6" t="inlineStr">
+        <v>3.5</v>
+      </c>
+      <c r="E14" s="90" t="inlineStr">
         <is>
           <t>BILLS</t>
         </is>
@@ -7182,8 +7210,8 @@
       </c>
       <c r="L14" s="17" t="n"/>
       <c r="M14" s="18" t="n"/>
-      <c r="N14" s="87" t="n"/>
-      <c r="O14" s="87" t="n"/>
+      <c r="N14" s="94" t="n"/>
+      <c r="O14" s="94" t="n"/>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="15" t="n"/>

</xml_diff>

<commit_message>
Add aditional test Excel file. Update existing Excel test file and pool.py.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -63,7 +63,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -134,6 +134,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="0000B0F0"/>
         <bgColor rgb="0000B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -486,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -710,6 +716,13 @@
     <xf numFmtId="49" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6767,9 +6780,9 @@
         </is>
       </c>
       <c r="D2" s="15" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
+        <v>1</v>
+      </c>
+      <c r="E2" s="95" t="inlineStr">
         <is>
           <t>BEARS</t>
         </is>
@@ -6796,13 +6809,13 @@
     <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="15" t="n"/>
       <c r="B3" s="15" t="n"/>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="95" t="inlineStr">
         <is>
           <t>LIONS</t>
         </is>
       </c>
       <c r="D3" s="15" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="89" t="inlineStr">
         <is>
@@ -6839,7 +6852,7 @@
       <c r="D4" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" s="96" t="inlineStr">
         <is>
           <t>FALCONS</t>
         </is>
@@ -6872,9 +6885,9 @@
         </is>
       </c>
       <c r="D5" s="15" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
+        <v>4</v>
+      </c>
+      <c r="E5" s="97" t="inlineStr">
         <is>
           <t>TEXANS</t>
         </is>
@@ -6909,7 +6922,7 @@
       <c r="D6" s="15" t="n">
         <v>2.5</v>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="E6" s="97" t="inlineStr">
         <is>
           <t>FOOTBALL TEAM</t>
         </is>
@@ -6942,9 +6955,9 @@
         </is>
       </c>
       <c r="D7" s="15" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1" t="inlineStr">
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="97" t="inlineStr">
         <is>
           <t>BROWNS</t>
         </is>
@@ -6971,13 +6984,13 @@
     <row r="8" ht="15.6" customHeight="1">
       <c r="A8" s="15" t="n"/>
       <c r="B8" s="15" t="n"/>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="96" t="inlineStr">
         <is>
           <t>RAVENS</t>
         </is>
       </c>
       <c r="D8" s="15" t="n">
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="E8" s="91" t="inlineStr">
         <is>
@@ -7012,9 +7025,9 @@
         </is>
       </c>
       <c r="D9" s="15" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
+        <v>7.5</v>
+      </c>
+      <c r="E9" s="97" t="inlineStr">
         <is>
           <t>BENGALS</t>
         </is>
@@ -7047,9 +7060,9 @@
         </is>
       </c>
       <c r="D10" s="15" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="E10" s="95" t="inlineStr">
         <is>
           <t>BRONCOS</t>
         </is>
@@ -7084,7 +7097,7 @@
       <c r="D11" s="15" t="n">
         <v>9.5</v>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="E11" s="95" t="inlineStr">
         <is>
           <t>JETS</t>
         </is>
@@ -7111,7 +7124,7 @@
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="15" t="n"/>
       <c r="B12" s="15" t="n"/>
-      <c r="C12" s="1" t="inlineStr">
+      <c r="C12" s="97" t="inlineStr">
         <is>
           <t>PACKERS</t>
         </is>
@@ -7146,13 +7159,13 @@
     <row r="13" ht="15.6" customHeight="1">
       <c r="A13" s="15" t="n"/>
       <c r="B13" s="15" t="n"/>
-      <c r="C13" s="1" t="inlineStr">
+      <c r="C13" s="97" t="inlineStr">
         <is>
           <t>RAMS</t>
         </is>
       </c>
       <c r="D13" s="15" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="92" t="inlineStr">
         <is>
@@ -7181,7 +7194,7 @@
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="15" t="n"/>
       <c r="B14" s="15" t="n"/>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" s="95" t="inlineStr">
         <is>
           <t>CHIEFS</t>
         </is>
@@ -7216,13 +7229,13 @@
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="15" t="n"/>
       <c r="B15" s="15" t="n"/>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" s="95" t="inlineStr">
         <is>
           <t>CARDINALS</t>
         </is>
       </c>
       <c r="D15" s="15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="92" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update Test Excel and pool.py files.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4770" yWindow="2685" windowWidth="28800" windowHeight="11370" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5055" yWindow="1845" windowWidth="28815" windowHeight="11370" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Week 4" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Week 5" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Week 6" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Week 7" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -63,7 +64,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill/>
     </fill>
@@ -122,6 +123,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor rgb="FFF4B084"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -492,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -674,6 +693,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -700,29 +742,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,7 +1147,7 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -1133,13 +1178,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="75" t="inlineStr">
+      <c r="C1" s="84" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="76" t="n"/>
-      <c r="E1" s="77" t="n"/>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="86" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1151,14 +1196,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="78" t="inlineStr">
+      <c r="I1" s="87" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="76" t="n"/>
-      <c r="K1" s="76" t="n"/>
-      <c r="L1" s="77" t="n"/>
+      <c r="J1" s="85" t="n"/>
+      <c r="K1" s="85" t="n"/>
+      <c r="L1" s="86" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -1540,7 +1585,7 @@
   </sheetPr>
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1564,11 +1609,11 @@
     <col width="13" customWidth="1" style="39" min="18" max="18"/>
     <col width="5.21875" customWidth="1" style="39" min="19" max="19"/>
     <col width="5" customWidth="1" style="39" min="20" max="20"/>
-    <col width="8.77734375" customWidth="1" style="39" min="21" max="51"/>
-    <col width="8.77734375" customWidth="1" style="39" min="52" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="21" max="52"/>
+    <col width="8.77734375" customWidth="1" style="39" min="53" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1579,13 +1624,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="79" t="inlineStr">
+      <c r="C1" s="88" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="80" t="n"/>
-      <c r="E1" s="81" t="n"/>
+      <c r="D1" s="89" t="n"/>
+      <c r="E1" s="90" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -1597,14 +1642,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="82" t="inlineStr">
+      <c r="I1" s="91" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="80" t="n"/>
-      <c r="K1" s="80" t="n"/>
-      <c r="L1" s="83" t="n"/>
+      <c r="J1" s="89" t="n"/>
+      <c r="K1" s="89" t="n"/>
+      <c r="L1" s="92" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -1619,7 +1664,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A2" s="15" t="n"/>
       <c r="B2" s="15" t="n"/>
       <c r="C2" s="22" t="inlineStr">
@@ -1675,7 +1720,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1731,7 +1776,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A4" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1787,7 +1832,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -1843,7 +1888,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -1899,7 +1944,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A7" s="15" t="n"/>
       <c r="B7" s="15" t="n"/>
       <c r="C7" s="23" t="inlineStr">
@@ -1953,13 +1998,13 @@
           <t>W</t>
         </is>
       </c>
-      <c r="P7" s="87" t="inlineStr">
+      <c r="P7" s="96" t="inlineStr">
         <is>
           <t>De predicts 49ers 27-20</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2015,7 +2060,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2071,7 +2116,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2127,7 +2172,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A11" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2183,7 +2228,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2239,7 +2284,7 @@
       </c>
       <c r="P12" s="58" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A13" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2295,7 +2340,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2351,7 +2396,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2407,7 +2452,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A16" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2463,7 +2508,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A17" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2519,7 +2564,7 @@
       </c>
       <c r="P17" s="58" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -2550,7 +2595,7 @@
       <c r="P18" s="58" t="n"/>
       <c r="Q18" s="58" t="n"/>
     </row>
-    <row r="19" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="19" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -2581,20 +2626,20 @@
       <c r="P19" s="58" t="n"/>
       <c r="Q19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
-      <c r="A20" s="84" t="inlineStr">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="97">
+      <c r="A20" s="93" t="inlineStr">
         <is>
           <t>DeM says the Super Bowl will be won by the Falcons</t>
         </is>
       </c>
-      <c r="B20" s="85" t="n"/>
-      <c r="C20" s="85" t="n"/>
-      <c r="D20" s="85" t="n"/>
-      <c r="E20" s="85" t="n"/>
-      <c r="F20" s="85" t="n"/>
-      <c r="G20" s="85" t="n"/>
-      <c r="H20" s="85" t="n"/>
-      <c r="I20" s="86" t="n"/>
+      <c r="B20" s="94" t="n"/>
+      <c r="C20" s="94" t="n"/>
+      <c r="D20" s="94" t="n"/>
+      <c r="E20" s="94" t="n"/>
+      <c r="F20" s="94" t="n"/>
+      <c r="G20" s="94" t="n"/>
+      <c r="H20" s="94" t="n"/>
+      <c r="I20" s="95" t="n"/>
       <c r="J20" s="31" t="n"/>
       <c r="K20" s="27" t="n"/>
       <c r="L20" s="31" t="inlineStr">
@@ -2616,7 +2661,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="21" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A21" s="34" t="inlineStr">
         <is>
           <t>playing against the</t>
@@ -2670,7 +2715,7 @@
   </sheetPr>
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="L19" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
@@ -2691,11 +2736,11 @@
     <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
     <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
     <col width="14.33203125" customWidth="1" style="39" min="18" max="19"/>
-    <col width="8.77734375" customWidth="1" style="39" min="20" max="50"/>
-    <col width="8.77734375" customWidth="1" style="39" min="51" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="20" max="51"/>
+    <col width="8.77734375" customWidth="1" style="39" min="52" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -2706,13 +2751,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="79" t="inlineStr">
+      <c r="C1" s="88" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="80" t="n"/>
-      <c r="E1" s="81" t="n"/>
+      <c r="D1" s="89" t="n"/>
+      <c r="E1" s="90" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -2724,14 +2769,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="82" t="inlineStr">
+      <c r="I1" s="91" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="80" t="n"/>
-      <c r="K1" s="80" t="n"/>
-      <c r="L1" s="83" t="n"/>
+      <c r="J1" s="89" t="n"/>
+      <c r="K1" s="89" t="n"/>
+      <c r="L1" s="92" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -2746,7 +2791,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A2" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2802,7 +2847,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2858,7 +2903,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A4" s="15" t="n"/>
       <c r="B4" s="15" t="inlineStr">
         <is>
@@ -2914,7 +2959,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A5" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -2970,7 +3015,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -3026,7 +3071,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A7" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3082,7 +3127,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3138,7 +3183,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A9" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3194,7 +3239,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A10" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3250,7 +3295,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
       <c r="C11" s="20" t="inlineStr">
@@ -3317,7 +3362,7 @@
       <c r="V11" s="58" t="n"/>
       <c r="W11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A12" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3384,7 +3429,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A13" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3451,7 +3496,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3507,7 +3552,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3563,7 +3608,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A16" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3619,7 +3664,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A17" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -3675,7 +3720,7 @@
       </c>
       <c r="P17" s="58" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -3706,7 +3751,7 @@
       <c r="P18" s="58" t="n"/>
       <c r="Q18" s="45" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -3740,7 +3785,7 @@
       <c r="S19" s="46" t="n"/>
       <c r="T19" s="46" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -3771,7 +3816,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="C21" s="27" t="n"/>
@@ -3819,7 +3864,7 @@
   </sheetPr>
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -3839,11 +3884,11 @@
     <col width="7.109375" customWidth="1" style="41" min="14" max="14"/>
     <col width="7.109375" customWidth="1" style="42" min="15" max="15"/>
     <col width="8.77734375" customWidth="1" style="43" min="16" max="17"/>
-    <col width="8.77734375" customWidth="1" style="39" min="18" max="48"/>
-    <col width="8.77734375" customWidth="1" style="39" min="49" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="18" max="49"/>
+    <col width="8.77734375" customWidth="1" style="39" min="50" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -3854,13 +3899,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="79" t="inlineStr">
+      <c r="C1" s="88" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="80" t="n"/>
-      <c r="E1" s="81" t="n"/>
+      <c r="D1" s="89" t="n"/>
+      <c r="E1" s="90" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -3872,14 +3917,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="82" t="inlineStr">
+      <c r="I1" s="91" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="80" t="n"/>
-      <c r="K1" s="80" t="n"/>
-      <c r="L1" s="83" t="n"/>
+      <c r="J1" s="89" t="n"/>
+      <c r="K1" s="89" t="n"/>
+      <c r="L1" s="92" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -3894,7 +3939,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A2" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -3950,7 +3995,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A3" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4006,7 +4051,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A4" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4062,7 +4107,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A5" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4118,7 +4163,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A6" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4174,7 +4219,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A7" s="61" t="n"/>
       <c r="B7" s="61" t="inlineStr">
         <is>
@@ -4230,7 +4275,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A8" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4286,7 +4331,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A9" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4342,7 +4387,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A10" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4398,7 +4443,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A11" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4454,7 +4499,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A12" s="61" t="n"/>
       <c r="B12" s="61" t="inlineStr">
         <is>
@@ -4510,7 +4555,7 @@
       </c>
       <c r="P12" s="58" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A13" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4566,7 +4611,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A14" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4622,7 +4667,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A15" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4678,7 +4723,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A16" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4734,7 +4779,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A17" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -4792,7 +4837,7 @@
       <c r="Q17" s="66" t="n"/>
       <c r="R17" s="66" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -4822,7 +4867,7 @@
       </c>
       <c r="P18" s="58" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -4853,7 +4898,7 @@
       <c r="P19" s="58" t="n"/>
       <c r="Q19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -4884,7 +4929,7 @@
       <c r="P20" s="58" t="n"/>
       <c r="Q20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="D21" s="26" t="n"/>
@@ -4929,7 +4974,7 @@
   </sheetPr>
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
@@ -4951,11 +4996,11 @@
     <col width="8.77734375" customWidth="1" style="43" min="16" max="16"/>
     <col width="14.33203125" customWidth="1" style="43" min="17" max="17"/>
     <col width="12.5546875" customWidth="1" style="39" min="18" max="18"/>
-    <col width="8.77734375" customWidth="1" style="39" min="19" max="49"/>
-    <col width="8.77734375" customWidth="1" style="39" min="50" max="16384"/>
+    <col width="8.77734375" customWidth="1" style="39" min="19" max="50"/>
+    <col width="8.77734375" customWidth="1" style="39" min="51" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="88" thickBot="1">
+    <row r="1" ht="16.15" customFormat="1" customHeight="1" s="97" thickBot="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
           <t>HM</t>
@@ -4966,13 +5011,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="79" t="inlineStr">
+      <c r="C1" s="88" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="80" t="n"/>
-      <c r="E1" s="81" t="n"/>
+      <c r="D1" s="89" t="n"/>
+      <c r="E1" s="90" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -4984,14 +5029,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="82" t="inlineStr">
+      <c r="I1" s="91" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="80" t="n"/>
-      <c r="K1" s="80" t="n"/>
-      <c r="L1" s="83" t="n"/>
+      <c r="J1" s="89" t="n"/>
+      <c r="K1" s="89" t="n"/>
+      <c r="L1" s="92" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="44" t="inlineStr">
         <is>
@@ -5006,7 +5051,7 @@
       <c r="P1" s="58" t="n"/>
       <c r="Q1" s="58" t="n"/>
     </row>
-    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="2" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A2" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5062,7 +5107,7 @@
       </c>
       <c r="P2" s="58" t="n"/>
     </row>
-    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="3" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A3" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5118,7 +5163,7 @@
       </c>
       <c r="P3" s="58" t="n"/>
     </row>
-    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="4" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A4" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5174,7 +5219,7 @@
       </c>
       <c r="P4" s="58" t="n"/>
     </row>
-    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="5" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A5" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5230,7 +5275,7 @@
       </c>
       <c r="P5" s="58" t="n"/>
     </row>
-    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="6" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A6" s="61" t="n"/>
       <c r="B6" s="15" t="inlineStr">
         <is>
@@ -5286,7 +5331,7 @@
       </c>
       <c r="P6" s="58" t="n"/>
     </row>
-    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="7" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A7" s="61" t="n"/>
       <c r="B7" s="15" t="inlineStr">
         <is>
@@ -5342,7 +5387,7 @@
       </c>
       <c r="P7" s="58" t="n"/>
     </row>
-    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="8" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A8" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5398,7 +5443,7 @@
       </c>
       <c r="P8" s="58" t="n"/>
     </row>
-    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="9" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A9" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5454,7 +5499,7 @@
       </c>
       <c r="P9" s="58" t="n"/>
     </row>
-    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="10" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A10" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5510,7 +5555,7 @@
       </c>
       <c r="P10" s="58" t="n"/>
     </row>
-    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="11" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A11" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5566,7 +5611,7 @@
       </c>
       <c r="P11" s="58" t="n"/>
     </row>
-    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="12" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A12" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5623,7 +5668,7 @@
       <c r="P12" s="58" t="n"/>
       <c r="T12" s="46" t="n"/>
     </row>
-    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="13" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A13" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5679,7 +5724,7 @@
       </c>
       <c r="P13" s="58" t="n"/>
     </row>
-    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="14" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A14" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5735,7 +5780,7 @@
       </c>
       <c r="P14" s="58" t="n"/>
     </row>
-    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="15" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A15" s="15" t="inlineStr">
         <is>
           <t>X</t>
@@ -5791,7 +5836,7 @@
       </c>
       <c r="P15" s="58" t="n"/>
     </row>
-    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="16" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A16" s="61" t="inlineStr">
         <is>
           <t>X</t>
@@ -5847,7 +5892,7 @@
       </c>
       <c r="P16" s="58" t="n"/>
     </row>
-    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="17" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A17" s="15" t="n"/>
       <c r="B17" s="15" t="n"/>
       <c r="C17" s="1" t="n"/>
@@ -5868,7 +5913,7 @@
       <c r="R17" s="66" t="n"/>
       <c r="T17" s="46" t="n"/>
     </row>
-    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="18" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A18" s="26" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
@@ -5898,7 +5943,7 @@
       </c>
       <c r="P18" s="58" t="n"/>
     </row>
-    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="19" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A19" s="30" t="n"/>
       <c r="B19" s="30" t="n"/>
       <c r="C19" s="31" t="n"/>
@@ -5928,7 +5973,7 @@
       </c>
       <c r="P19" s="58" t="n"/>
     </row>
-    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="20" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A20" s="15" t="n"/>
       <c r="B20" s="15" t="n"/>
       <c r="C20" s="1" t="n"/>
@@ -5958,7 +6003,7 @@
       </c>
       <c r="P20" s="58" t="n"/>
     </row>
-    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="88">
+    <row r="21" ht="15.6" customFormat="1" customHeight="1" s="97">
       <c r="A21" s="26" t="n"/>
       <c r="B21" s="26" t="n"/>
       <c r="C21" s="27" t="n"/>
@@ -6012,7 +6057,7 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -6043,13 +6088,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="75" t="inlineStr">
+      <c r="C1" s="84" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="76" t="n"/>
-      <c r="E1" s="77" t="n"/>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="86" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6061,14 +6106,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="78" t="inlineStr">
+      <c r="I1" s="87" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="76" t="n"/>
-      <c r="K1" s="76" t="n"/>
-      <c r="L1" s="77" t="n"/>
+      <c r="J1" s="85" t="n"/>
+      <c r="K1" s="85" t="n"/>
+      <c r="L1" s="86" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -6702,7 +6747,7 @@
   </sheetPr>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6733,13 +6778,13 @@
           <t>DE</t>
         </is>
       </c>
-      <c r="C1" s="75" t="inlineStr">
+      <c r="C1" s="84" t="inlineStr">
         <is>
           <t>AMERICA'S LINE</t>
         </is>
       </c>
-      <c r="D1" s="76" t="n"/>
-      <c r="E1" s="77" t="n"/>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="86" t="n"/>
       <c r="F1" s="9" t="inlineStr">
         <is>
           <t>HM</t>
@@ -6751,14 +6796,14 @@
         </is>
       </c>
       <c r="H1" s="11" t="n"/>
-      <c r="I1" s="78" t="inlineStr">
+      <c r="I1" s="87" t="inlineStr">
         <is>
           <t>ACTUAL SCORES</t>
         </is>
       </c>
-      <c r="J1" s="76" t="n"/>
-      <c r="K1" s="76" t="n"/>
-      <c r="L1" s="77" t="n"/>
+      <c r="J1" s="85" t="n"/>
+      <c r="K1" s="85" t="n"/>
+      <c r="L1" s="86" t="n"/>
       <c r="M1" s="11" t="n"/>
       <c r="N1" s="12" t="inlineStr">
         <is>
@@ -6774,7 +6819,7 @@
     <row r="2" ht="15.6" customHeight="1">
       <c r="A2" s="15" t="n"/>
       <c r="B2" s="15" t="n"/>
-      <c r="C2" s="89" t="inlineStr">
+      <c r="C2" s="75" t="inlineStr">
         <is>
           <t>PANTHERS</t>
         </is>
@@ -6782,7 +6827,7 @@
       <c r="D2" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="95" t="inlineStr">
+      <c r="E2" s="81" t="inlineStr">
         <is>
           <t>BEARS</t>
         </is>
@@ -6809,7 +6854,7 @@
     <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="15" t="n"/>
       <c r="B3" s="15" t="n"/>
-      <c r="C3" s="95" t="inlineStr">
+      <c r="C3" s="81" t="inlineStr">
         <is>
           <t>LIONS</t>
         </is>
@@ -6817,7 +6862,7 @@
       <c r="D3" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="89" t="inlineStr">
+      <c r="E3" s="75" t="inlineStr">
         <is>
           <t>JAGUARS</t>
         </is>
@@ -6844,7 +6889,7 @@
     <row r="4" ht="15.6" customHeight="1">
       <c r="A4" s="15" t="n"/>
       <c r="B4" s="15" t="n"/>
-      <c r="C4" s="90" t="inlineStr">
+      <c r="C4" s="76" t="inlineStr">
         <is>
           <t>VIKINGS</t>
         </is>
@@ -6852,7 +6897,7 @@
       <c r="D4" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E4" s="96" t="inlineStr">
+      <c r="E4" s="82" t="inlineStr">
         <is>
           <t>FALCONS</t>
         </is>
@@ -6879,7 +6924,7 @@
     <row r="5" ht="15.6" customHeight="1">
       <c r="A5" s="15" t="n"/>
       <c r="B5" s="15" t="n"/>
-      <c r="C5" s="91" t="inlineStr">
+      <c r="C5" s="77" t="inlineStr">
         <is>
           <t>TITANS</t>
         </is>
@@ -6887,7 +6932,7 @@
       <c r="D5" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="97" t="inlineStr">
+      <c r="E5" s="83" t="inlineStr">
         <is>
           <t>TEXANS</t>
         </is>
@@ -6914,7 +6959,7 @@
     <row r="6" ht="15.6" customHeight="1">
       <c r="A6" s="15" t="n"/>
       <c r="B6" s="15" t="n"/>
-      <c r="C6" s="92" t="inlineStr">
+      <c r="C6" s="78" t="inlineStr">
         <is>
           <t>GIANTS</t>
         </is>
@@ -6922,7 +6967,7 @@
       <c r="D6" s="15" t="n">
         <v>2.5</v>
       </c>
-      <c r="E6" s="97" t="inlineStr">
+      <c r="E6" s="83" t="inlineStr">
         <is>
           <t>FOOTBALL TEAM</t>
         </is>
@@ -6949,7 +6994,7 @@
     <row r="7" ht="15.6" customHeight="1">
       <c r="A7" s="15" t="n"/>
       <c r="B7" s="15" t="n"/>
-      <c r="C7" s="91" t="inlineStr">
+      <c r="C7" s="77" t="inlineStr">
         <is>
           <t>STEELERS</t>
         </is>
@@ -6957,7 +7002,7 @@
       <c r="D7" s="15" t="n">
         <v>3.5</v>
       </c>
-      <c r="E7" s="97" t="inlineStr">
+      <c r="E7" s="83" t="inlineStr">
         <is>
           <t>BROWNS</t>
         </is>
@@ -6984,7 +7029,7 @@
     <row r="8" ht="15.6" customHeight="1">
       <c r="A8" s="15" t="n"/>
       <c r="B8" s="15" t="n"/>
-      <c r="C8" s="96" t="inlineStr">
+      <c r="C8" s="82" t="inlineStr">
         <is>
           <t>RAVENS</t>
         </is>
@@ -6992,7 +7037,7 @@
       <c r="D8" s="15" t="n">
         <v>9.5</v>
       </c>
-      <c r="E8" s="91" t="inlineStr">
+      <c r="E8" s="77" t="inlineStr">
         <is>
           <t>EAGLES</t>
         </is>
@@ -7019,7 +7064,7 @@
     <row r="9" ht="15.6" customHeight="1">
       <c r="A9" s="15" t="n"/>
       <c r="B9" s="15" t="n"/>
-      <c r="C9" s="92" t="inlineStr">
+      <c r="C9" s="78" t="inlineStr">
         <is>
           <t>COLTS</t>
         </is>
@@ -7027,7 +7072,7 @@
       <c r="D9" s="15" t="n">
         <v>7.5</v>
       </c>
-      <c r="E9" s="97" t="inlineStr">
+      <c r="E9" s="83" t="inlineStr">
         <is>
           <t>BENGALS</t>
         </is>
@@ -7054,7 +7099,7 @@
     <row r="10" ht="15.6" customHeight="1">
       <c r="A10" s="15" t="n"/>
       <c r="B10" s="15" t="n"/>
-      <c r="C10" s="91" t="inlineStr">
+      <c r="C10" s="77" t="inlineStr">
         <is>
           <t>PATRIOTS</t>
         </is>
@@ -7062,7 +7107,7 @@
       <c r="D10" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="95" t="inlineStr">
+      <c r="E10" s="81" t="inlineStr">
         <is>
           <t>BRONCOS</t>
         </is>
@@ -7089,7 +7134,7 @@
     <row r="11" ht="15.6" customHeight="1">
       <c r="A11" s="15" t="n"/>
       <c r="B11" s="15" t="n"/>
-      <c r="C11" s="92" t="inlineStr">
+      <c r="C11" s="78" t="inlineStr">
         <is>
           <t>DOLPHINS</t>
         </is>
@@ -7097,7 +7142,7 @@
       <c r="D11" s="15" t="n">
         <v>9.5</v>
       </c>
-      <c r="E11" s="95" t="inlineStr">
+      <c r="E11" s="81" t="inlineStr">
         <is>
           <t>JETS</t>
         </is>
@@ -7124,7 +7169,7 @@
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="15" t="n"/>
       <c r="B12" s="15" t="n"/>
-      <c r="C12" s="97" t="inlineStr">
+      <c r="C12" s="83" t="inlineStr">
         <is>
           <t>PACKERS</t>
         </is>
@@ -7132,7 +7177,7 @@
       <c r="D12" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="92" t="inlineStr">
+      <c r="E12" s="78" t="inlineStr">
         <is>
           <t>BUCCANEERS</t>
         </is>
@@ -7159,7 +7204,7 @@
     <row r="13" ht="15.6" customHeight="1">
       <c r="A13" s="15" t="n"/>
       <c r="B13" s="15" t="n"/>
-      <c r="C13" s="97" t="inlineStr">
+      <c r="C13" s="83" t="inlineStr">
         <is>
           <t>RAMS</t>
         </is>
@@ -7167,7 +7212,7 @@
       <c r="D13" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="E13" s="92" t="inlineStr">
+      <c r="E13" s="78" t="inlineStr">
         <is>
           <t>49ERS</t>
         </is>
@@ -7188,13 +7233,13 @@
       </c>
       <c r="L13" s="17" t="n"/>
       <c r="M13" s="18" t="n"/>
-      <c r="N13" s="93" t="n"/>
-      <c r="O13" s="94" t="n"/>
+      <c r="N13" s="79" t="n"/>
+      <c r="O13" s="80" t="n"/>
     </row>
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="15" t="n"/>
       <c r="B14" s="15" t="n"/>
-      <c r="C14" s="95" t="inlineStr">
+      <c r="C14" s="81" t="inlineStr">
         <is>
           <t>CHIEFS</t>
         </is>
@@ -7202,7 +7247,7 @@
       <c r="D14" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="E14" s="90" t="inlineStr">
+      <c r="E14" s="76" t="inlineStr">
         <is>
           <t>BILLS</t>
         </is>
@@ -7223,13 +7268,13 @@
       </c>
       <c r="L14" s="17" t="n"/>
       <c r="M14" s="18" t="n"/>
-      <c r="N14" s="94" t="n"/>
-      <c r="O14" s="94" t="n"/>
+      <c r="N14" s="80" t="n"/>
+      <c r="O14" s="80" t="n"/>
     </row>
     <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="15" t="n"/>
       <c r="B15" s="15" t="n"/>
-      <c r="C15" s="95" t="inlineStr">
+      <c r="C15" s="81" t="inlineStr">
         <is>
           <t>CARDINALS</t>
         </is>
@@ -7237,7 +7282,7 @@
       <c r="D15" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="92" t="inlineStr">
+      <c r="E15" s="78" t="inlineStr">
         <is>
           <t>COWBOYS</t>
         </is>
@@ -7258,8 +7303,8 @@
       </c>
       <c r="L15" s="17" t="n"/>
       <c r="M15" s="18" t="n"/>
-      <c r="N15" s="93" t="n"/>
-      <c r="O15" s="94" t="n"/>
+      <c r="N15" s="79" t="n"/>
+      <c r="O15" s="80" t="n"/>
     </row>
     <row r="16" ht="15.6" customHeight="1">
       <c r="A16" s="15" t="n"/>
@@ -7382,4 +7427,694 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="4" customWidth="1" min="1" max="2"/>
+    <col width="17.44140625" customWidth="1" min="3" max="3"/>
+    <col width="6.44140625" customWidth="1" min="4" max="4"/>
+    <col width="17.44140625" customWidth="1" min="5" max="5"/>
+    <col width="4" customWidth="1" min="6" max="7"/>
+    <col width="1.88671875" customWidth="1" min="8" max="8"/>
+    <col width="5.44140625" customWidth="1" min="9" max="9"/>
+    <col width="5" customWidth="1" min="10" max="10"/>
+    <col width="5.44140625" customWidth="1" min="11" max="11"/>
+    <col width="5" customWidth="1" min="12" max="12"/>
+    <col width="1.88671875" customWidth="1" min="13" max="13"/>
+    <col width="7.109375" customWidth="1" min="14" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.15" customHeight="1" thickBot="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="C1" s="84" t="inlineStr">
+        <is>
+          <t>AMERICA'S LINE</t>
+        </is>
+      </c>
+      <c r="D1" s="85" t="n"/>
+      <c r="E1" s="86" t="n"/>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="H1" s="11" t="n"/>
+      <c r="I1" s="87" t="inlineStr">
+        <is>
+          <t>ACTUAL SCORES</t>
+        </is>
+      </c>
+      <c r="J1" s="85" t="n"/>
+      <c r="K1" s="85" t="n"/>
+      <c r="L1" s="86" t="n"/>
+      <c r="M1" s="11" t="n"/>
+      <c r="N1" s="12" t="inlineStr">
+        <is>
+          <t>HM</t>
+        </is>
+      </c>
+      <c r="O1" s="13" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.6" customHeight="1">
+      <c r="A2" s="15" t="n"/>
+      <c r="B2" s="15" t="n"/>
+      <c r="C2" s="98" t="inlineStr">
+        <is>
+          <t>EAGLES</t>
+        </is>
+      </c>
+      <c r="D2" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>GIANTS</t>
+        </is>
+      </c>
+      <c r="F2" s="55" t="n"/>
+      <c r="G2" s="55" t="n"/>
+      <c r="H2" s="16" t="n"/>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="J2" s="17" t="n"/>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>NYG</t>
+        </is>
+      </c>
+      <c r="L2" s="17" t="n"/>
+      <c r="M2" s="18" t="n"/>
+      <c r="N2" s="61" t="n"/>
+      <c r="O2" s="70" t="n"/>
+    </row>
+    <row r="3" ht="15.6" customHeight="1">
+      <c r="A3" s="15" t="n"/>
+      <c r="B3" s="15" t="n"/>
+      <c r="C3" s="4" t="inlineStr">
+        <is>
+          <t>BROWNS</t>
+        </is>
+      </c>
+      <c r="D3" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="98" t="inlineStr">
+        <is>
+          <t>BENGALS</t>
+        </is>
+      </c>
+      <c r="F3" s="21" t="n"/>
+      <c r="G3" s="15" t="n"/>
+      <c r="H3" s="16" t="n"/>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="J3" s="17" t="n"/>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>CIN</t>
+        </is>
+      </c>
+      <c r="L3" s="17" t="n"/>
+      <c r="M3" s="18" t="n"/>
+      <c r="N3" s="61" t="n"/>
+      <c r="O3" s="19" t="n"/>
+    </row>
+    <row r="4" ht="15.6" customHeight="1">
+      <c r="A4" s="15" t="n"/>
+      <c r="B4" s="15" t="n"/>
+      <c r="C4" s="104" t="inlineStr">
+        <is>
+          <t>COWBOYS</t>
+        </is>
+      </c>
+      <c r="D4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="98" t="inlineStr">
+        <is>
+          <t>FOOTBALL TEAM</t>
+        </is>
+      </c>
+      <c r="F4" s="21" t="n"/>
+      <c r="G4" s="15" t="n"/>
+      <c r="H4" s="16" t="n"/>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="J4" s="17" t="n"/>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="L4" s="17" t="n"/>
+      <c r="M4" s="18" t="n"/>
+      <c r="N4" s="61" t="n"/>
+      <c r="O4" s="19" t="n"/>
+    </row>
+    <row r="5" ht="15.6" customHeight="1">
+      <c r="A5" s="15" t="n"/>
+      <c r="B5" s="15" t="n"/>
+      <c r="C5" s="105" t="inlineStr">
+        <is>
+          <t>FALCONS</t>
+        </is>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="99" t="inlineStr">
+        <is>
+          <t>LIONS</t>
+        </is>
+      </c>
+      <c r="F5" s="21" t="n"/>
+      <c r="G5" s="15" t="n"/>
+      <c r="H5" s="16" t="n"/>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="J5" s="17" t="n"/>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="L5" s="17" t="n"/>
+      <c r="M5" s="18" t="n"/>
+      <c r="N5" s="61" t="n"/>
+      <c r="O5" s="19" t="n"/>
+    </row>
+    <row r="6" ht="15.6" customHeight="1">
+      <c r="A6" s="15" t="n"/>
+      <c r="B6" s="15" t="n"/>
+      <c r="C6" s="100" t="inlineStr">
+        <is>
+          <t>SAINTS</t>
+        </is>
+      </c>
+      <c r="D6" s="15" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E6" s="105" t="inlineStr">
+        <is>
+          <t>PANTHERS</t>
+        </is>
+      </c>
+      <c r="F6" s="21" t="n"/>
+      <c r="G6" s="15" t="n"/>
+      <c r="H6" s="16" t="n"/>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="J6" s="17" t="n"/>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>CAR</t>
+        </is>
+      </c>
+      <c r="L6" s="17" t="n"/>
+      <c r="M6" s="18" t="n"/>
+      <c r="N6" s="61" t="n"/>
+      <c r="O6" s="19" t="n"/>
+    </row>
+    <row r="7" ht="15.6" customHeight="1">
+      <c r="A7" s="15" t="n"/>
+      <c r="B7" s="15" t="n"/>
+      <c r="C7" s="99" t="inlineStr">
+        <is>
+          <t>BILLS</t>
+        </is>
+      </c>
+      <c r="D7" s="15" t="n">
+        <v>13.5</v>
+      </c>
+      <c r="E7" s="105" t="inlineStr">
+        <is>
+          <t>JETS</t>
+        </is>
+      </c>
+      <c r="F7" s="21" t="n"/>
+      <c r="G7" s="15" t="n"/>
+      <c r="H7" s="16" t="n"/>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>BUF</t>
+        </is>
+      </c>
+      <c r="J7" s="17" t="n"/>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>NYJ</t>
+        </is>
+      </c>
+      <c r="L7" s="17" t="n"/>
+      <c r="M7" s="18" t="n"/>
+      <c r="N7" s="61" t="n"/>
+      <c r="O7" s="61" t="n"/>
+    </row>
+    <row r="8" ht="15.6" customHeight="1">
+      <c r="A8" s="15" t="n"/>
+      <c r="B8" s="15" t="n"/>
+      <c r="C8" s="106" t="inlineStr">
+        <is>
+          <t>PACKERS</t>
+        </is>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="99" t="inlineStr">
+        <is>
+          <t>TEXANS</t>
+        </is>
+      </c>
+      <c r="F8" s="57" t="n"/>
+      <c r="G8" s="15" t="n"/>
+      <c r="H8" s="16" t="n"/>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="J8" s="17" t="n"/>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>HOU</t>
+        </is>
+      </c>
+      <c r="L8" s="17" t="n"/>
+      <c r="M8" s="18" t="n"/>
+      <c r="N8" s="61" t="n"/>
+      <c r="O8" s="19" t="n"/>
+    </row>
+    <row r="9" ht="15.6" customHeight="1">
+      <c r="A9" s="15" t="n"/>
+      <c r="B9" s="15" t="n"/>
+      <c r="C9" s="107" t="inlineStr">
+        <is>
+          <t>STEELERS</t>
+        </is>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="99" t="inlineStr">
+        <is>
+          <t>TITANS</t>
+        </is>
+      </c>
+      <c r="F9" s="21" t="n"/>
+      <c r="G9" s="15" t="n"/>
+      <c r="H9" s="16" t="n"/>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>PIT</t>
+        </is>
+      </c>
+      <c r="J9" s="17" t="n"/>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>TEN</t>
+        </is>
+      </c>
+      <c r="L9" s="17" t="n"/>
+      <c r="M9" s="18" t="n"/>
+      <c r="N9" s="61" t="n"/>
+      <c r="O9" s="19" t="n"/>
+    </row>
+    <row r="10" ht="15.6" customHeight="1">
+      <c r="A10" s="15" t="n"/>
+      <c r="B10" s="15" t="n"/>
+      <c r="C10" s="105" t="inlineStr">
+        <is>
+          <t>SEAHAWKS</t>
+        </is>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E10" s="100" t="inlineStr">
+        <is>
+          <t>CARDINALS</t>
+        </is>
+      </c>
+      <c r="F10" s="21" t="n"/>
+      <c r="G10" s="15" t="n"/>
+      <c r="H10" s="16" t="n"/>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>SEA</t>
+        </is>
+      </c>
+      <c r="J10" s="17" t="n"/>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>ARI</t>
+        </is>
+      </c>
+      <c r="L10" s="17" t="n"/>
+      <c r="M10" s="18" t="n"/>
+      <c r="N10" s="61" t="n"/>
+      <c r="O10" s="19" t="n"/>
+    </row>
+    <row r="11" ht="15.6" customHeight="1">
+      <c r="A11" s="15" t="n"/>
+      <c r="B11" s="15" t="n"/>
+      <c r="C11" s="107" t="inlineStr">
+        <is>
+          <t>PATRIOTS</t>
+        </is>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="100" t="inlineStr">
+        <is>
+          <t>49ERS</t>
+        </is>
+      </c>
+      <c r="F11" s="57" t="n"/>
+      <c r="G11" s="15" t="n"/>
+      <c r="H11" s="16" t="n"/>
+      <c r="I11" s="2" t="inlineStr">
+        <is>
+          <t>NE</t>
+        </is>
+      </c>
+      <c r="J11" s="17" t="n"/>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>SF</t>
+        </is>
+      </c>
+      <c r="L11" s="17" t="n"/>
+      <c r="M11" s="18" t="n"/>
+      <c r="N11" s="61" t="n"/>
+      <c r="O11" s="19" t="n"/>
+    </row>
+    <row r="12" ht="15.6" customHeight="1">
+      <c r="A12" s="15" t="n"/>
+      <c r="B12" s="15" t="n"/>
+      <c r="C12" s="99" t="inlineStr">
+        <is>
+          <t>CHIEFS</t>
+        </is>
+      </c>
+      <c r="D12" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="E12" s="107" t="inlineStr">
+        <is>
+          <t>BRONCOS</t>
+        </is>
+      </c>
+      <c r="F12" s="21" t="n"/>
+      <c r="G12" s="15" t="n"/>
+      <c r="H12" s="16" t="n"/>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>KC</t>
+        </is>
+      </c>
+      <c r="J12" s="17" t="n"/>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>DEN</t>
+        </is>
+      </c>
+      <c r="L12" s="17" t="n"/>
+      <c r="M12" s="18" t="n"/>
+      <c r="N12" s="61" t="n"/>
+      <c r="O12" s="19" t="n"/>
+    </row>
+    <row r="13" ht="15.6" customHeight="1">
+      <c r="A13" s="15" t="n"/>
+      <c r="B13" s="15" t="n"/>
+      <c r="C13" s="105" t="inlineStr">
+        <is>
+          <t>CHARGERS</t>
+        </is>
+      </c>
+      <c r="D13" s="15" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E13" s="100" t="inlineStr">
+        <is>
+          <t>JAGUARS</t>
+        </is>
+      </c>
+      <c r="F13" s="21" t="n"/>
+      <c r="G13" s="15" t="n"/>
+      <c r="H13" s="16" t="n"/>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="J13" s="17" t="n"/>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>JAX</t>
+        </is>
+      </c>
+      <c r="L13" s="17" t="n"/>
+      <c r="M13" s="18" t="n"/>
+      <c r="N13" s="61" t="n"/>
+      <c r="O13" s="19" t="n"/>
+    </row>
+    <row r="14" ht="15.6" customHeight="1">
+      <c r="A14" s="15" t="n"/>
+      <c r="B14" s="15" t="n"/>
+      <c r="C14" s="100" t="inlineStr">
+        <is>
+          <t>BUCCANEERS</t>
+        </is>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="104" t="inlineStr">
+        <is>
+          <t>RAIDERS</t>
+        </is>
+      </c>
+      <c r="F14" s="21" t="n"/>
+      <c r="G14" s="15" t="n"/>
+      <c r="H14" s="16" t="n"/>
+      <c r="I14" s="2" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="J14" s="17" t="n"/>
+      <c r="K14" s="5" t="inlineStr">
+        <is>
+          <t>LV</t>
+        </is>
+      </c>
+      <c r="L14" s="17" t="n"/>
+      <c r="M14" s="18" t="n"/>
+      <c r="N14" s="102" t="n"/>
+      <c r="O14" s="102" t="n"/>
+    </row>
+    <row r="15" ht="15.6" customHeight="1">
+      <c r="A15" s="15" t="n"/>
+      <c r="B15" s="15" t="n"/>
+      <c r="C15" s="107" t="inlineStr">
+        <is>
+          <t>RAMS</t>
+        </is>
+      </c>
+      <c r="D15" s="15" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E15" s="100" t="inlineStr">
+        <is>
+          <t>BEARS</t>
+        </is>
+      </c>
+      <c r="F15" s="21" t="n"/>
+      <c r="G15" s="15" t="n"/>
+      <c r="H15" s="16" t="n"/>
+      <c r="I15" s="2" t="inlineStr">
+        <is>
+          <t>LAR</t>
+        </is>
+      </c>
+      <c r="J15" s="17" t="n"/>
+      <c r="K15" s="2" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="L15" s="17" t="n"/>
+      <c r="M15" s="18" t="n"/>
+      <c r="N15" s="103" t="n"/>
+      <c r="O15" s="102" t="n"/>
+    </row>
+    <row r="16" ht="15.6" customHeight="1">
+      <c r="A16" s="15" t="n"/>
+      <c r="B16" s="15" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="15" t="n"/>
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="21" t="n"/>
+      <c r="G16" s="15" t="n"/>
+      <c r="H16" s="16" t="n"/>
+      <c r="I16" s="2" t="n"/>
+      <c r="J16" s="17" t="n"/>
+      <c r="K16" s="2" t="n"/>
+      <c r="L16" s="17" t="n"/>
+      <c r="M16" s="18" t="n"/>
+      <c r="N16" s="24" t="n"/>
+      <c r="O16" s="24" t="n"/>
+    </row>
+    <row r="17" ht="15.6" customHeight="1">
+      <c r="A17" s="15" t="n"/>
+      <c r="B17" s="15" t="n"/>
+      <c r="C17" s="1" t="n"/>
+      <c r="D17" s="15" t="n"/>
+      <c r="E17" s="1" t="n"/>
+      <c r="F17" s="21" t="n"/>
+      <c r="G17" s="15" t="n"/>
+      <c r="H17" s="16" t="n"/>
+      <c r="I17" s="2" t="n"/>
+      <c r="J17" s="17" t="n"/>
+      <c r="K17" s="2" t="n"/>
+      <c r="L17" s="17" t="n"/>
+      <c r="M17" s="18" t="n"/>
+      <c r="N17" s="61" t="n"/>
+      <c r="O17" s="19" t="n"/>
+    </row>
+    <row r="18" ht="15.6" customHeight="1">
+      <c r="A18" s="26" t="n"/>
+      <c r="B18" s="26" t="n"/>
+      <c r="C18" s="67" t="n"/>
+      <c r="D18" s="56" t="n"/>
+      <c r="E18" s="68" t="n"/>
+      <c r="F18" s="28" t="n"/>
+      <c r="G18" s="26" t="n"/>
+      <c r="H18" s="29" t="n"/>
+      <c r="I18" s="5" t="n"/>
+      <c r="J18" s="17" t="n"/>
+      <c r="K18" s="5" t="n"/>
+      <c r="L18" s="17" t="inlineStr">
+        <is>
+          <t>SUB</t>
+        </is>
+      </c>
+      <c r="M18" s="16" t="n"/>
+      <c r="N18" s="19" t="n"/>
+      <c r="O18" s="19" t="n"/>
+    </row>
+    <row r="19" ht="15.6" customHeight="1">
+      <c r="A19" s="26" t="n"/>
+      <c r="B19" s="26" t="n"/>
+      <c r="C19" s="67" t="n"/>
+      <c r="D19" s="56" t="n"/>
+      <c r="E19" s="68" t="n"/>
+      <c r="F19" s="28" t="n"/>
+      <c r="G19" s="26" t="n"/>
+      <c r="H19" s="29" t="n"/>
+      <c r="I19" s="5" t="n"/>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="5" t="n"/>
+      <c r="L19" s="17" t="inlineStr">
+        <is>
+          <t>WK</t>
+        </is>
+      </c>
+      <c r="M19" s="16" t="n"/>
+      <c r="N19" s="19" t="n"/>
+      <c r="O19" s="19" t="n"/>
+    </row>
+    <row r="20" ht="15.6" customHeight="1">
+      <c r="A20" s="26" t="n"/>
+      <c r="B20" s="26" t="n"/>
+      <c r="C20" s="67" t="n"/>
+      <c r="D20" s="56" t="n"/>
+      <c r="E20" s="68" t="n"/>
+      <c r="F20" s="28" t="n"/>
+      <c r="G20" s="26" t="n"/>
+      <c r="H20" s="29" t="n"/>
+      <c r="I20" s="5" t="n"/>
+      <c r="J20" s="17" t="n"/>
+      <c r="K20" s="5" t="n"/>
+      <c r="L20" s="31" t="inlineStr">
+        <is>
+          <t>YTD</t>
+        </is>
+      </c>
+      <c r="M20" s="16" t="n"/>
+      <c r="N20" s="19" t="n"/>
+      <c r="O20" s="19" t="n"/>
+    </row>
+    <row r="21" ht="15.6" customHeight="1">
+      <c r="A21" s="61" t="n"/>
+      <c r="B21" s="61" t="n"/>
+      <c r="C21" s="4" t="n"/>
+      <c r="D21" s="15" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="69" t="n"/>
+      <c r="G21" s="61" t="n"/>
+      <c r="H21" s="16" t="n"/>
+      <c r="I21" s="5" t="n"/>
+      <c r="J21" s="17" t="n"/>
+      <c r="K21" s="5" t="n"/>
+      <c r="L21" s="17" t="n"/>
+      <c r="M21" s="16" t="n"/>
+      <c r="N21" s="19" t="n"/>
+      <c r="O21" s="19" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Test Excel and pool.py files. Refactor pool.py to replace static values for variables on the number of Thurs and number of Sat games.
</commit_message>
<xml_diff>
--- a/Family Football Pool Testing.xlsx
+++ b/Family Football Pool Testing.xlsx
@@ -529,7 +529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -796,6 +796,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7573,7 +7576,7 @@
     <row r="3" ht="15.6" customHeight="1">
       <c r="A3" s="15" t="n"/>
       <c r="B3" s="15" t="n"/>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="112" t="inlineStr">
         <is>
           <t>BROWNS</t>
         </is>
@@ -7581,7 +7584,7 @@
       <c r="D3" s="15" t="n">
         <v>3.5</v>
       </c>
-      <c r="E3" s="83" t="inlineStr">
+      <c r="E3" s="113" t="inlineStr">
         <is>
           <t>BENGALS</t>
         </is>
@@ -7859,7 +7862,7 @@
         </is>
       </c>
       <c r="D11" s="15" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E11" s="112" t="inlineStr">
         <is>
@@ -7894,7 +7897,7 @@
         </is>
       </c>
       <c r="D12" s="15" t="n">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="E12" s="111" t="inlineStr">
         <is>
@@ -7999,7 +8002,7 @@
         </is>
       </c>
       <c r="D15" s="15" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="112" t="inlineStr">
         <is>

</xml_diff>